<commit_message>
Added Get-FormFactors to the list
</commit_message>
<xml_diff>
--- a/Matt's code compendium.xlsx
+++ b/Matt's code compendium.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="435" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{770EE1CE-533E-4158-8EFB-4CF92645BECD}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mseng3\Git\code-compendium\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2294E386-FC6C-459F-96C9-53CA6DF114FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,11 +18,11 @@
     <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$83</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sheet1 (2)'!$B$1:$F$83</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sheet1 (3)'!$B$1:$F$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sheet1 (2)'!$B$1:$F$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sheet1 (3)'!$B$1:$F$84</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="169">
   <si>
     <t>Name</t>
   </si>
@@ -528,13 +533,25 @@
   </si>
   <si>
     <t>[Validate-Win7ESUCompat](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Validate-Win7ESUCompat)</t>
+  </si>
+  <si>
+    <t>Gets form factor and other info (WMI Win32_SystemEnclosure and Win32_ComputerSystem classes) from remote endpoints</t>
+  </si>
+  <si>
+    <t>[Get-FormFactors](https://github.com/engrit-illinois/Get-FormFactors)</t>
+  </si>
+  <si>
+    <t>Get-FormFactors</t>
+  </si>
+  <si>
+    <t>https://github.com/engrit-illinois/Get-FormFactors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -904,14 +921,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="51.140625" customWidth="1"/>
@@ -922,7 +939,7 @@
     <col min="7" max="7" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -945,7 +962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -968,7 +985,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -991,7 +1008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1014,7 +1031,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1037,7 +1054,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1060,7 +1077,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -1083,7 +1100,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1106,7 +1123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1129,7 +1146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -1152,7 +1169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1175,7 +1192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -1198,61 +1215,61 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75">
-      <c r="A14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="75">
-      <c r="A15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>55</v>
@@ -1261,47 +1278,47 @@
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="45">
-      <c r="A17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
@@ -1313,18 +1330,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>11</v>
@@ -1336,61 +1353,61 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45">
-      <c r="A20" s="1" t="s">
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30">
-      <c r="A21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>77</v>
@@ -1405,41 +1422,41 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30">
-      <c r="A23" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>11</v>
@@ -1451,38 +1468,38 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45">
-      <c r="A25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>24</v>
@@ -1491,90 +1508,90 @@
         <v>11</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30">
-      <c r="A27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="45">
-      <c r="A28" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45">
-      <c r="A29" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>105</v>
@@ -1589,154 +1606,168 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45">
-      <c r="A31" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="45">
-      <c r="A32" s="1" t="s">
+      <c r="F32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="45">
-      <c r="A33" s="1" t="s">
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="45">
-      <c r="A34" s="1" t="s">
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1745,7 +1776,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1754,7 +1785,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1763,7 +1794,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1772,7 +1803,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1781,7 +1812,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1790,10 +1821,19 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G83" xr:uid="{82CE97CC-043E-4C7B-A7B6-0AF71D812FA2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G83">
-      <sortCondition ref="A1:A83"/>
+  <autoFilter ref="A1:G84" xr:uid="{82CE97CC-043E-4C7B-A7B6-0AF71D812FA2}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G84">
+      <sortCondition ref="A1:A84"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -1804,28 +1844,29 @@
     <hyperlink ref="C4" r:id="rId5" xr:uid="{050CA958-EF94-48AF-BB20-B08B5B0DD70C}"/>
     <hyperlink ref="C8" r:id="rId6" xr:uid="{C70CC111-F139-4058-9797-A90AD8076F0A}"/>
     <hyperlink ref="C10" r:id="rId7" xr:uid="{3D4046BF-E0B8-40CF-A9BB-A3A95A78C044}"/>
-    <hyperlink ref="C13" r:id="rId8" xr:uid="{A2EF598B-1569-462A-A492-0AB216B6D4E9}"/>
-    <hyperlink ref="C14" r:id="rId9" xr:uid="{F0DA93D9-E5AD-48BE-A149-EBF4DF8E7665}"/>
-    <hyperlink ref="C15" r:id="rId10" xr:uid="{16E345CA-E21F-4BB0-A698-2872A48AFFAC}"/>
-    <hyperlink ref="C16" r:id="rId11" xr:uid="{8CF6CA95-B5A3-4C35-B517-AC7B44C00F9A}"/>
-    <hyperlink ref="C17" r:id="rId12" xr:uid="{144A0DEE-F894-43FD-A2B0-43E0D6AE94F5}"/>
-    <hyperlink ref="C18" r:id="rId13" xr:uid="{55681E8C-673D-45BA-8A29-B0C4ACDA12E2}"/>
-    <hyperlink ref="C19" r:id="rId14" xr:uid="{49BE894C-326D-4DB0-82FA-39B905015181}"/>
-    <hyperlink ref="C20" r:id="rId15" xr:uid="{E4315478-7499-49A9-8B30-981239230CE9}"/>
-    <hyperlink ref="C22" r:id="rId16" xr:uid="{8F4F0F83-DB3C-45CB-94A8-0F4C2222E6EF}"/>
-    <hyperlink ref="C23" r:id="rId17" xr:uid="{A1A26D75-1A49-433B-B577-268734D44491}"/>
-    <hyperlink ref="C24" r:id="rId18" xr:uid="{2BC41496-E6C4-4CDC-BFF6-278E052F6205}"/>
-    <hyperlink ref="C25" r:id="rId19" xr:uid="{F6D2B089-DF2F-4010-A266-504E831BDAA7}"/>
-    <hyperlink ref="C26" r:id="rId20" xr:uid="{5F7E1424-B0D3-4404-B86D-E34579B07B5F}"/>
-    <hyperlink ref="C27" r:id="rId21" xr:uid="{8EDB5CF4-FC6D-4EB6-969D-53C54B38E866}"/>
-    <hyperlink ref="C28" r:id="rId22" xr:uid="{2305894F-D802-47D3-97D5-6E48AB36BD4F}"/>
-    <hyperlink ref="C29" r:id="rId23" xr:uid="{76C27548-09D0-4920-9D3E-2D1A6EF707D8}"/>
-    <hyperlink ref="C30" r:id="rId24" xr:uid="{B3F6CC47-EC5A-43F3-89EF-A9F3FB60EDFB}"/>
-    <hyperlink ref="C31" r:id="rId25" xr:uid="{5FB4A99D-840F-4419-8025-6BAF388F82A9}"/>
-    <hyperlink ref="C33" r:id="rId26" xr:uid="{E639F861-6CD3-421D-AA1F-64D661DD5049}"/>
-    <hyperlink ref="C34" r:id="rId27" xr:uid="{A2C3ED0B-852C-4BB9-887A-8137A387AD12}"/>
-    <hyperlink ref="C35" r:id="rId28" xr:uid="{A52D8E08-A6A8-4806-B4B0-9F279442EB75}"/>
-    <hyperlink ref="C21" r:id="rId29" xr:uid="{BD152848-19FA-4790-A66D-1E337E80DCA6}"/>
+    <hyperlink ref="C14" r:id="rId8" xr:uid="{A2EF598B-1569-462A-A492-0AB216B6D4E9}"/>
+    <hyperlink ref="C15" r:id="rId9" xr:uid="{F0DA93D9-E5AD-48BE-A149-EBF4DF8E7665}"/>
+    <hyperlink ref="C16" r:id="rId10" xr:uid="{16E345CA-E21F-4BB0-A698-2872A48AFFAC}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{8CF6CA95-B5A3-4C35-B517-AC7B44C00F9A}"/>
+    <hyperlink ref="C18" r:id="rId12" xr:uid="{144A0DEE-F894-43FD-A2B0-43E0D6AE94F5}"/>
+    <hyperlink ref="C19" r:id="rId13" xr:uid="{55681E8C-673D-45BA-8A29-B0C4ACDA12E2}"/>
+    <hyperlink ref="C20" r:id="rId14" xr:uid="{49BE894C-326D-4DB0-82FA-39B905015181}"/>
+    <hyperlink ref="C21" r:id="rId15" xr:uid="{E4315478-7499-49A9-8B30-981239230CE9}"/>
+    <hyperlink ref="C23" r:id="rId16" xr:uid="{8F4F0F83-DB3C-45CB-94A8-0F4C2222E6EF}"/>
+    <hyperlink ref="C24" r:id="rId17" xr:uid="{A1A26D75-1A49-433B-B577-268734D44491}"/>
+    <hyperlink ref="C25" r:id="rId18" xr:uid="{2BC41496-E6C4-4CDC-BFF6-278E052F6205}"/>
+    <hyperlink ref="C26" r:id="rId19" xr:uid="{F6D2B089-DF2F-4010-A266-504E831BDAA7}"/>
+    <hyperlink ref="C27" r:id="rId20" xr:uid="{5F7E1424-B0D3-4404-B86D-E34579B07B5F}"/>
+    <hyperlink ref="C28" r:id="rId21" xr:uid="{8EDB5CF4-FC6D-4EB6-969D-53C54B38E866}"/>
+    <hyperlink ref="C29" r:id="rId22" xr:uid="{2305894F-D802-47D3-97D5-6E48AB36BD4F}"/>
+    <hyperlink ref="C30" r:id="rId23" xr:uid="{76C27548-09D0-4920-9D3E-2D1A6EF707D8}"/>
+    <hyperlink ref="C31" r:id="rId24" xr:uid="{B3F6CC47-EC5A-43F3-89EF-A9F3FB60EDFB}"/>
+    <hyperlink ref="C32" r:id="rId25" xr:uid="{5FB4A99D-840F-4419-8025-6BAF388F82A9}"/>
+    <hyperlink ref="C34" r:id="rId26" xr:uid="{E639F861-6CD3-421D-AA1F-64D661DD5049}"/>
+    <hyperlink ref="C35" r:id="rId27" xr:uid="{A2C3ED0B-852C-4BB9-887A-8137A387AD12}"/>
+    <hyperlink ref="C36" r:id="rId28" xr:uid="{A52D8E08-A6A8-4806-B4B0-9F279442EB75}"/>
+    <hyperlink ref="C22" r:id="rId29" xr:uid="{BD152848-19FA-4790-A66D-1E337E80DCA6}"/>
+    <hyperlink ref="C13" r:id="rId30" xr:uid="{025ED15E-271F-4436-9336-80F003A5B9E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1833,14 +1874,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4FA528-FCA3-42D6-B177-1CC7649F1D01}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="51.140625" customWidth="1"/>
@@ -1852,7 +1893,7 @@
     <col min="8" max="8" width="106.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>130</v>
       </c>
@@ -1878,9 +1919,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45">
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f>CONCATENATE("[",G2,"](",H2,")")</f>
+        <f t="shared" ref="A2:A36" si="0">CONCATENATE("[",G2,"](",H2,")")</f>
         <v>[Recycle-EWSGuestAccounts](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Recycle-EWSGuestAccounts)</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1905,9 +1946,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
-        <f>CONCATENATE("[",G3,"](",H3,")")</f>
+        <f t="shared" si="0"/>
         <v>[create-role-based-ad-accounts-and-groups](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/create-role-based-ad-accounts-and-groups)</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1932,9 +1973,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
-        <f>CONCATENATE("[",G4,"](",H4,")")</f>
+        <f t="shared" si="0"/>
         <v>[Create-ICTDocClassAccounts](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Create-ICTDocClassAccounts)</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1959,9 +2000,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
-        <f>CONCATENATE("[",G5,"](",H5,")")</f>
+        <f t="shared" si="0"/>
         <v>[get-lens-info](https://gitlab.engr.illinois.edu/engrit-epm/sccm-ts-scripts/-/blob/master/get-lens-info.ps1)</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1986,9 +2027,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
-        <f>CONCATENATE("[",G6,"](",H6,")")</f>
+        <f t="shared" si="0"/>
         <v>[post-to-slack](https://gitlab.engr.illinois.edu/engrit-epm/sccm-ts-scripts/-/blob/master/post-to-slack.ps1)</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2013,9 +2054,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
-        <f>CONCATENATE("[",G7,"](",H7,")")</f>
+        <f t="shared" si="0"/>
         <v>[post-to-teams](https://gitlab.engr.illinois.edu/engrit-epm/sccm-ts-scripts/-/blob/master/post-to-teams.ps1)</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2040,9 +2081,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
-        <f>CONCATENATE("[",G8,"](",H8,")")</f>
+        <f t="shared" si="0"/>
         <v>[Get-Sessions](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Get-Sessions)</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2067,9 +2108,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30">
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
-        <f>CONCATENATE("[",G9,"](",H9,")")</f>
+        <f t="shared" si="0"/>
         <v>[Get-ComputersBySessionState](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Get-ComputersBySessionState)</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2094,9 +2135,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
-        <f>CONCATENATE("[",G10,"](",H10,")")</f>
+        <f t="shared" si="0"/>
         <v>[Get-Model](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Get-Model)</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2121,9 +2162,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
-        <f>CONCATENATE("[",G11,"](",H11,")")</f>
+        <f t="shared" si="0"/>
         <v>[Get-DiskSpace](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Get-DiskSpace)</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2148,9 +2189,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
-        <f>CONCATENATE("[",G12,"](",H12,")")</f>
+        <f t="shared" si="0"/>
         <v>[Get-UptimeHistory](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Get-UptimeHistory)</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2175,67 +2216,66 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30">
-      <c r="A13" s="1" t="str">
-        <f>CONCATENATE("[",G13,"](",H13,")")</f>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[misc-handy-powershell-examples](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/misc-handy-powershell-examples)</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="75">
-      <c r="A14" s="1" t="str">
-        <f>CONCATENATE("[",G14,"](",H14,")")</f>
+    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[org-shared-deployments](https://gitlab.engr.illinois.edu/engrit-epm/org-shared-deployments)</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="75">
-      <c r="A15" s="1" t="str">
-        <f>CONCATENATE("[",G15,"](",H15,")")</f>
-        <v>[Audit-StaleADComputersInOU](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Audit-StaleADComputersInOU)</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>55</v>
@@ -2244,55 +2284,55 @@
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[Audit-StaleADComputersInOU](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Audit-StaleADComputersInOU)</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="1" t="str">
-        <f>CONCATENATE("[",G16,"](",H16,")")</f>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[bcdedit-revert-uefi-gpt-boot-order](https://github.com/mmseng/bcdedit-revert-uefi-gpt-boot-order)</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="45">
-      <c r="A17" s="1" t="str">
-        <f>CONCATENATE("[",G17,"](",H17,")")</f>
-        <v>[Compare-AssignmentRevisions](https://gitlab.engr.illinois.edu/engrit-epm/compare-assignmentrevisions)</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
@@ -2304,22 +2344,22 @@
         <v>26</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
-        <f>CONCATENATE("[",G18,"](",H18,")")</f>
-        <v>[count-ad-objects](https://gitlab.engr.illinois.edu/engrit-epm/sccm-ts-scripts/-/blob/master/count-ad-objects.ps1)</v>
+        <f t="shared" si="0"/>
+        <v>[Compare-AssignmentRevisions](https://gitlab.engr.illinois.edu/engrit-epm/compare-assignmentrevisions)</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -2331,73 +2371,73 @@
         <v>26</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[count-ad-objects](https://gitlab.engr.illinois.edu/engrit-epm/sccm-ts-scripts/-/blob/master/count-ad-objects.ps1)</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45">
-      <c r="A19" s="1" t="str">
-        <f>CONCATENATE("[",G19,"](",H19,")")</f>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[Covidize-LabOU](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Covidize-LabOU)</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45">
-      <c r="A20" s="1" t="str">
-        <f>CONCATENATE("[",G20,"](",H20,")")</f>
+    <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[force-mecm-baseline-evaluation](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/force-mecm-baseline-evaluation)</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30">
-      <c r="A21" s="1" t="str">
-        <f>CONCATENATE("[",G21,"](",H21,")")</f>
-        <v>[force-software-center-assignment-evaluation](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/force-software-center-assignment-evaluation)</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>77</v>
@@ -2412,49 +2452,49 @@
         <v>13</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[force-software-center-assignment-evaluation](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/force-software-center-assignment-evaluation)</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45">
-      <c r="A22" s="1" t="str">
-        <f>CONCATENATE("[",G22,"](",H22,")")</f>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[Export-PrintServerPrinters](https://gitlab.engr.illinois.edu/engrit-epm/export-printserverprinters)</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30">
-      <c r="A23" s="1" t="str">
-        <f>CONCATENATE("[",G23,"](",H23,")")</f>
-        <v>[Get-AppSupersedence](https://gitlab.engr.illinois.edu/engrit-epm/get-appsupersedence)</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
@@ -2466,46 +2506,46 @@
         <v>26</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[Get-AppSupersedence](https://gitlab.engr.illinois.edu/engrit-epm/get-appsupersedence)</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30">
-      <c r="A24" s="1" t="str">
-        <f>CONCATENATE("[",G24,"](",H24,")")</f>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[Get-CobblerSystems](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Get-CobblerSystems)</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="45">
-      <c r="A25" s="1" t="str">
-        <f>CONCATENATE("[",G25,"](",H25,")")</f>
-        <v>[Get-SccmEngrPrefixes](https://gitlab.engr.illinois.edu/engrit-epm/get-sccmengrprefixes)</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>24</v>
@@ -2514,106 +2554,106 @@
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[Get-SccmEngrPrefixes](https://gitlab.engr.illinois.edu/engrit-epm/get-sccmengrprefixes)</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="60">
-      <c r="A26" s="1" t="str">
-        <f>CONCATENATE("[",G26,"](",H26,")")</f>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[Helptools Importer](https://gitlab.engr.illinois.edu/engrit-epm/helptools-importer)</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30">
-      <c r="A27" s="1" t="str">
-        <f>CONCATENATE("[",G27,"](",H27,")")</f>
+    <row r="28" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[msi-app-uninstall](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/blob/master/msi-app-uninstall/msi-app-uninstall.ps1)</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45">
-      <c r="A28" s="1" t="str">
-        <f>CONCATENATE("[",G28,"](",H28,")")</f>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[Ping-All](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Ping-All)</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="45">
-      <c r="A29" s="1" t="str">
-        <f>CONCATENATE("[",G29,"](",H29,")")</f>
-        <v>[Ping-OverTime](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Ping-OverTime)</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>105</v>
@@ -2628,185 +2668,202 @@
         <v>13</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[Ping-OverTime](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Ping-OverTime)</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30">
-      <c r="A30" s="1" t="str">
-        <f>CONCATENATE("[",G30,"](",H30,")")</f>
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[powershell-profile-example](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/powershell-profile-example)</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="45">
-      <c r="A31" s="1" t="str">
-        <f>CONCATENATE("[",G31,"](",H31,")")</f>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[PrinterStatus](https://helptools.engrit.illinois.edu/tools/printerstatus/)</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="1" t="s">
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="45">
-      <c r="A32" s="1" t="str">
-        <f>CONCATENATE("[",G32,"](",H32,")")</f>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[PWResetV2](Contact for more information.)</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45">
-      <c r="A33" s="1" t="str">
-        <f>CONCATENATE("[",G33,"](",H33,")")</f>
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[Report-AMTStatus](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Report-AMTStatus)</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="45">
-      <c r="A34" s="1" t="str">
-        <f>CONCATENATE("[",G34,"](",H34,")")</f>
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[Report-ProductVersion](https://gitlab.engr.illinois.edu/engrit-epm/report-productversion)</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30">
-      <c r="A35" s="1" t="str">
-        <f>CONCATENATE("[",G35,"](",H35,")")</f>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>[Validate-Win7ESUCompat](https://gitlab.engr.illinois.edu/oesr/official_engrit_script_repo/-/tree/master/Validate-Win7ESUCompat)</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2816,7 +2873,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2826,7 +2883,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2836,7 +2893,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2846,7 +2903,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2856,7 +2913,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2866,8 +2923,18 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:F83" xr:uid="{82CE97CC-043E-4C7B-A7B6-0AF71D812FA2}"/>
+  <autoFilter ref="B1:F84" xr:uid="{82CE97CC-043E-4C7B-A7B6-0AF71D812FA2}"/>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" xr:uid="{FDECDAAD-C15C-412C-B4FB-010F4894D2D3}"/>
     <hyperlink ref="H12" r:id="rId2" xr:uid="{ECDAF0A3-C2F4-4D5C-9531-74AEBF11A75B}"/>
@@ -2876,28 +2943,28 @@
     <hyperlink ref="H4" r:id="rId5" xr:uid="{EC917C74-04F2-48AB-A931-B9B6EF615A61}"/>
     <hyperlink ref="H8" r:id="rId6" xr:uid="{C98BE662-6DBD-4268-9BE4-8D0ED1483953}"/>
     <hyperlink ref="H10" r:id="rId7" xr:uid="{B6FD1961-F01F-456E-B971-D7DDFCE83C15}"/>
-    <hyperlink ref="H13" r:id="rId8" xr:uid="{C1265EBE-E4C1-4D92-B2CC-32DC1412B285}"/>
-    <hyperlink ref="H14" r:id="rId9" xr:uid="{87B94590-93E5-4825-91F8-EF93820E1EAA}"/>
-    <hyperlink ref="H15" r:id="rId10" xr:uid="{BCC3FFF6-57B6-4BE7-812D-92B37A584393}"/>
-    <hyperlink ref="H16" r:id="rId11" xr:uid="{4789D2CF-2E5E-4201-B888-862E626AF9EF}"/>
-    <hyperlink ref="H17" r:id="rId12" xr:uid="{AF8D1BBC-9C5B-4E5A-89CE-1EB6F9CE61F4}"/>
-    <hyperlink ref="H18" r:id="rId13" xr:uid="{BBAC9AB1-8529-42B4-B122-CE32BDE6350C}"/>
-    <hyperlink ref="H19" r:id="rId14" xr:uid="{0AF81495-3886-44F8-B090-3E52D0E0B8C6}"/>
-    <hyperlink ref="H20" r:id="rId15" xr:uid="{E8DAF02D-FE43-491A-9667-4FB5BD3BE49B}"/>
-    <hyperlink ref="H22" r:id="rId16" xr:uid="{E659F9E6-662B-473B-9D34-AAB589AE254C}"/>
-    <hyperlink ref="H23" r:id="rId17" xr:uid="{9BD995EC-89C0-41B9-B7C6-1A64FF7A045D}"/>
-    <hyperlink ref="H24" r:id="rId18" xr:uid="{D41B5390-38A5-4E70-A4D7-FE553CD6306E}"/>
-    <hyperlink ref="H25" r:id="rId19" xr:uid="{2352F780-054C-4FA8-AB6E-3146B4A356FB}"/>
-    <hyperlink ref="H26" r:id="rId20" xr:uid="{CE1F0AA1-EFAE-4386-B9B3-6DFED380517C}"/>
-    <hyperlink ref="H27" r:id="rId21" xr:uid="{F1479A20-FC66-4C19-8F8F-7DCA1C493FD5}"/>
-    <hyperlink ref="H28" r:id="rId22" xr:uid="{055E0E90-FC70-4C3D-975A-ABEE0009AD26}"/>
-    <hyperlink ref="H29" r:id="rId23" xr:uid="{8831A775-C401-4690-91DC-9A0F580153AA}"/>
-    <hyperlink ref="H30" r:id="rId24" xr:uid="{2F0B024F-9CA3-48E9-B153-53EDA89D4B18}"/>
-    <hyperlink ref="H31" r:id="rId25" xr:uid="{5C7FE53B-F13E-4FE8-A0FE-4964E559FC8B}"/>
-    <hyperlink ref="H33" r:id="rId26" xr:uid="{CC84DCCC-8EF6-4EE6-B0B7-686B507958EB}"/>
-    <hyperlink ref="H34" r:id="rId27" xr:uid="{71467E69-68D4-4D6D-9A11-970143B84F6B}"/>
-    <hyperlink ref="H35" r:id="rId28" xr:uid="{24504841-FADD-41FA-825B-25DE5A2B990E}"/>
-    <hyperlink ref="H21" r:id="rId29" xr:uid="{8FE319D7-71F5-4252-B2B9-AA961AA9FEFF}"/>
+    <hyperlink ref="H14" r:id="rId8" xr:uid="{C1265EBE-E4C1-4D92-B2CC-32DC1412B285}"/>
+    <hyperlink ref="H15" r:id="rId9" xr:uid="{87B94590-93E5-4825-91F8-EF93820E1EAA}"/>
+    <hyperlink ref="H16" r:id="rId10" xr:uid="{BCC3FFF6-57B6-4BE7-812D-92B37A584393}"/>
+    <hyperlink ref="H17" r:id="rId11" xr:uid="{4789D2CF-2E5E-4201-B888-862E626AF9EF}"/>
+    <hyperlink ref="H18" r:id="rId12" xr:uid="{AF8D1BBC-9C5B-4E5A-89CE-1EB6F9CE61F4}"/>
+    <hyperlink ref="H19" r:id="rId13" xr:uid="{BBAC9AB1-8529-42B4-B122-CE32BDE6350C}"/>
+    <hyperlink ref="H20" r:id="rId14" xr:uid="{0AF81495-3886-44F8-B090-3E52D0E0B8C6}"/>
+    <hyperlink ref="H21" r:id="rId15" xr:uid="{E8DAF02D-FE43-491A-9667-4FB5BD3BE49B}"/>
+    <hyperlink ref="H23" r:id="rId16" xr:uid="{E659F9E6-662B-473B-9D34-AAB589AE254C}"/>
+    <hyperlink ref="H24" r:id="rId17" xr:uid="{9BD995EC-89C0-41B9-B7C6-1A64FF7A045D}"/>
+    <hyperlink ref="H25" r:id="rId18" xr:uid="{D41B5390-38A5-4E70-A4D7-FE553CD6306E}"/>
+    <hyperlink ref="H26" r:id="rId19" xr:uid="{2352F780-054C-4FA8-AB6E-3146B4A356FB}"/>
+    <hyperlink ref="H27" r:id="rId20" xr:uid="{CE1F0AA1-EFAE-4386-B9B3-6DFED380517C}"/>
+    <hyperlink ref="H28" r:id="rId21" xr:uid="{F1479A20-FC66-4C19-8F8F-7DCA1C493FD5}"/>
+    <hyperlink ref="H29" r:id="rId22" xr:uid="{055E0E90-FC70-4C3D-975A-ABEE0009AD26}"/>
+    <hyperlink ref="H30" r:id="rId23" xr:uid="{8831A775-C401-4690-91DC-9A0F580153AA}"/>
+    <hyperlink ref="H31" r:id="rId24" xr:uid="{2F0B024F-9CA3-48E9-B153-53EDA89D4B18}"/>
+    <hyperlink ref="H32" r:id="rId25" xr:uid="{5C7FE53B-F13E-4FE8-A0FE-4964E559FC8B}"/>
+    <hyperlink ref="H34" r:id="rId26" xr:uid="{CC84DCCC-8EF6-4EE6-B0B7-686B507958EB}"/>
+    <hyperlink ref="H35" r:id="rId27" xr:uid="{71467E69-68D4-4D6D-9A11-970143B84F6B}"/>
+    <hyperlink ref="H36" r:id="rId28" xr:uid="{24504841-FADD-41FA-825B-25DE5A2B990E}"/>
+    <hyperlink ref="H22" r:id="rId29" xr:uid="{8FE319D7-71F5-4252-B2B9-AA961AA9FEFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2905,14 +2972,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4545F2-B552-4015-9470-F7966E57D856}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.85546875" customWidth="1"/>
     <col min="2" max="2" width="51.140625" customWidth="1"/>
@@ -2922,7 +2989,7 @@
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>130</v>
       </c>
@@ -2942,7 +3009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>131</v>
       </c>
@@ -2962,7 +3029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>132</v>
       </c>
@@ -2982,7 +3049,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>133</v>
       </c>
@@ -3002,7 +3069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>134</v>
       </c>
@@ -3022,7 +3089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>135</v>
       </c>
@@ -3042,7 +3109,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>136</v>
       </c>
@@ -3062,7 +3129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>137</v>
       </c>
@@ -3082,7 +3149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60">
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>138</v>
       </c>
@@ -3102,7 +3169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>139</v>
       </c>
@@ -3122,7 +3189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>140</v>
       </c>
@@ -3142,7 +3209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>141</v>
       </c>
@@ -3162,52 +3229,52 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="75">
-      <c r="A14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="75">
-      <c r="A15" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>55</v>
@@ -3216,41 +3283,41 @@
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="45">
-      <c r="A17" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
@@ -3262,15 +3329,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -3282,52 +3349,52 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="45">
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60">
-      <c r="A20" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="60">
-      <c r="A21" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>77</v>
@@ -3342,35 +3409,35 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45">
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45">
-      <c r="A23" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
@@ -3382,32 +3449,32 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45">
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45">
-      <c r="A25" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>24</v>
@@ -3416,78 +3483,78 @@
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60">
-      <c r="A27" s="1" t="s">
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="45">
-      <c r="A28" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="45">
-      <c r="A29" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>105</v>
@@ -3502,135 +3569,147 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="60">
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="45">
-      <c r="A31" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="45">
-      <c r="A32" s="1" t="s">
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="45">
-      <c r="A33" s="1" t="s">
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45">
-      <c r="A34" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="60">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3638,7 +3717,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3646,7 +3725,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3654,7 +3733,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3662,7 +3741,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3670,7 +3749,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3678,8 +3757,16 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:F83" xr:uid="{82CE97CC-043E-4C7B-A7B6-0AF71D812FA2}"/>
+  <autoFilter ref="B1:F84" xr:uid="{82CE97CC-043E-4C7B-A7B6-0AF71D812FA2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>